<commit_message>
Duk Handout and Powerpoint refinements
</commit_message>
<xml_diff>
--- a/AWL/Kostenrechnung/01BÜB/03_BÜB Übungsbeispiele_AB.xlsx
+++ b/AWL/Kostenrechnung/01BÜB/03_BÜB Übungsbeispiele_AB.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_School\BS3\AWL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_School\BS3repo\AWL\Kostenrechnung\01BÜB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3296A62C-E2C6-40C1-B47D-4908F87029D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B54CC3F-3B54-4631-AD47-1BF175E0C32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16185" yWindow="15" windowWidth="16170" windowHeight="16905" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AB1" sheetId="4" r:id="rId1"/>
     <sheet name="AB2" sheetId="6" r:id="rId2"/>
-    <sheet name="AB3" sheetId="9" r:id="rId3"/>
-    <sheet name="BÜB-Vorlage" sheetId="10" r:id="rId4"/>
+    <sheet name="Lernen" sheetId="11" r:id="rId3"/>
+    <sheet name="AB3" sheetId="9" r:id="rId4"/>
+    <sheet name="BÜB-Vorlage" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>ÜBUNG 1</t>
   </si>
@@ -505,6 +506,9 @@
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -521,9 +525,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -871,43 +872,43 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="6" width="20.6640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.8" x14ac:dyDescent="0.65">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -927,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
@@ -941,7 +942,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
@@ -955,7 +956,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -969,7 +970,7 @@
         <v>18500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
@@ -983,7 +984,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
@@ -997,7 +998,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="19" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="19" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="19" t="s">
         <v>17</v>
       </c>
@@ -1053,7 +1054,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="19" t="s">
         <v>18</v>
       </c>
@@ -1067,7 +1068,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="10" t="s">
         <v>36</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>9700</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="10" t="s">
         <v>37</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>27500</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="10" t="s">
         <v>38</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="10" t="s">
         <v>39</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="10"/>
       <c r="B19" s="7"/>
       <c r="C19" s="13"/>
@@ -1131,7 +1132,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10"/>
       <c r="B20" s="8"/>
       <c r="C20" s="14"/>
@@ -1139,7 +1140,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="10"/>
       <c r="B21" s="9">
         <f>SUM(B5:B20)</f>
@@ -1162,16 +1163,16 @@
         <v>153500</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="21">
         <f>B21+C21+D21</f>
         <v>307500</v>
@@ -1180,7 +1181,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="22"/>
       <c r="C25" s="11" t="s">
         <v>41</v>
@@ -1190,7 +1191,7 @@
         <v>236.15384615384616</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="21">
         <f>F21+E21</f>
         <v>307500</v>
@@ -1203,7 +1204,7 @@
         <v>172.47191011235955</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="C27" s="11" t="s">
         <v>43</v>
       </c>
@@ -1227,11 +1228,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB4BFDB-FDC0-49A6-9362-D50EA8155B24}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F21" sqref="A4:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
@@ -1239,32 +1240,32 @@
     <col min="4" max="6" width="20.6640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.8" x14ac:dyDescent="0.65">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1299,7 +1300,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1315,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1344,7 +1345,7 @@
       </c>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -1359,7 +1360,7 @@
         <v>17400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1374,7 +1375,7 @@
         <v>32800</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="5" t="s">
         <v>26</v>
       </c>
@@ -1404,7 +1405,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -1418,7 +1419,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1433,7 +1434,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1448,7 +1449,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="10" t="s">
         <v>46</v>
       </c>
@@ -1478,7 +1479,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="10" t="s">
         <v>48</v>
       </c>
@@ -1494,7 +1495,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="10" t="s">
         <v>47</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="10" t="s">
         <v>52</v>
       </c>
@@ -1524,7 +1525,7 @@
         <v>6640</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="10"/>
       <c r="B21" s="15">
         <f t="shared" ref="B21:E21" si="0">SUM(B5:B20)</f>
@@ -1547,45 +1548,45 @@
         <v>140340</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A24" s="23">
         <f>B21+C21+D21</f>
         <v>468140</v>
       </c>
       <c r="B24" s="16"/>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="25">
         <f>F21*100/E5</f>
         <v>59.974358974358971</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A25" s="23">
         <f>F21+E21</f>
         <v>468140</v>
       </c>
       <c r="B25" s="16"/>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="25">
         <f>F21*100/(E8+E18+E19)</f>
         <v>149.61620469083155</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A26" s="17"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="25">
         <f>F21*100/E21</f>
         <v>42.812690665039661</v>
       </c>
@@ -1601,46 +1602,397 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24959781-B9BF-4FD0-AFB0-244DE1986297}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.38671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="96.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" ht="19.8" x14ac:dyDescent="0.65">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
+        <v>234000</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13">
+        <v>234000</v>
+      </c>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4">
+        <v>9000</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10200</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4">
+        <v>77800</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13">
+        <v>77800</v>
+      </c>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4">
+        <v>17400</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
+        <v>17400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4">
+        <v>32800</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13">
+        <v>32800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9300</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4">
+        <v>8300</v>
+      </c>
+      <c r="C11" s="13">
+        <f>B11*-1</f>
+        <v>-8300</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13">
+        <f>B11*0.8</f>
+        <v>6640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4">
+        <v>7900</v>
+      </c>
+      <c r="C12" s="13">
+        <f>-B12</f>
+        <v>-7900</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="4">
+        <v>20300</v>
+      </c>
+      <c r="C13" s="13">
+        <f>-B13</f>
+        <v>-20300</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13">
+        <v>5000</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13">
+        <v>15000</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13">
+        <v>24000</v>
+      </c>
+      <c r="E16" s="13">
+        <f>8000</f>
+        <v>8000</v>
+      </c>
+      <c r="F16" s="13">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13">
+        <v>24000</v>
+      </c>
+      <c r="E17" s="13">
+        <v>8000</v>
+      </c>
+      <c r="F17" s="13">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14">
+        <f>B11*0.8</f>
+        <v>6640</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14">
+        <f>B11*0.8</f>
+        <v>6640</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="A19" s="10"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15">
+        <f>SUM(C11:C18)</f>
+        <v>-36500</v>
+      </c>
+      <c r="D19" s="15">
+        <f>SUM(D14:D18)</f>
+        <v>74640</v>
+      </c>
+      <c r="E19" s="15">
+        <f>SUM(E3:E18)</f>
+        <v>327800</v>
+      </c>
+      <c r="F19" s="15">
+        <f>SUM(F3:F18)</f>
+        <v>146980</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19.8" x14ac:dyDescent="0.65">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.5">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
+      <c r="A22" s="23"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
+      <c r="A23" s="23"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0760A8DD-D161-4C8E-AFB9-1B8FBA91A797}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="6" width="20.6640625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-    </row>
-    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.8" x14ac:dyDescent="0.65">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1660,7 +2012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -1675,7 +2027,7 @@
       </c>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
@@ -1690,7 +2042,7 @@
       </c>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
@@ -1705,7 +2057,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1720,7 +2072,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="5" t="s">
         <v>33</v>
       </c>
@@ -1735,7 +2087,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1750,7 +2102,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
@@ -1765,7 +2117,7 @@
         <v>8600</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
@@ -1780,7 +2132,7 @@
         <v>18200</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="10" t="s">
         <v>50</v>
       </c>
@@ -1797,7 +2149,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="10" t="s">
         <v>51</v>
       </c>
@@ -1811,7 +2163,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14"/>
@@ -1819,7 +2171,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="10"/>
       <c r="B16" s="9">
         <f>SUM(B5:B15)</f>
@@ -1842,49 +2194,49 @@
         <v>112800</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="8.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-    </row>
-    <row r="19" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A19" s="24">
         <f>B16+C16+D16</f>
         <v>490800</v>
       </c>
       <c r="B19" s="16"/>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="25">
         <f>F16*100/E5</f>
         <v>51.272727272727273</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A20" s="24">
         <f>E16+F16</f>
         <v>490800</v>
       </c>
       <c r="B20" s="16"/>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="25">
         <f>F16*100/(E6+E13)</f>
         <v>71.392405063291136</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="17.7" x14ac:dyDescent="0.6">
       <c r="A21" s="17"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="25">
         <f>F16*100/E16</f>
         <v>29.841269841269842</v>
       </c>
@@ -1898,7 +2250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB0727C-7670-40D0-BAEC-760703D75EC3}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1909,7 +2261,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="26.5546875" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
@@ -1917,17 +2269,17 @@
     <col min="4" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="3" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+    </row>
+    <row r="3" spans="1:6" ht="19.8" x14ac:dyDescent="0.65">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1947,7 +2299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="13"/>
@@ -1955,7 +2307,7 @@
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A5" s="5"/>
       <c r="B5" s="4"/>
       <c r="C5" s="13"/>
@@ -1963,7 +2315,7 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A6" s="5"/>
       <c r="B6" s="4"/>
       <c r="C6" s="13"/>
@@ -1971,7 +2323,7 @@
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A7" s="5"/>
       <c r="B7" s="4"/>
       <c r="C7" s="13"/>
@@ -1979,7 +2331,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A8" s="5"/>
       <c r="B8" s="4"/>
       <c r="C8" s="13"/>
@@ -1987,7 +2339,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A9" s="5"/>
       <c r="B9" s="4"/>
       <c r="C9" s="13"/>
@@ -1995,7 +2347,7 @@
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A10" s="5"/>
       <c r="B10" s="4"/>
       <c r="C10" s="13"/>
@@ -2003,7 +2355,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A11" s="5"/>
       <c r="B11" s="4"/>
       <c r="C11" s="13"/>
@@ -2011,7 +2363,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A12" s="5"/>
       <c r="B12" s="4"/>
       <c r="C12" s="13"/>
@@ -2019,7 +2371,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A13" s="5"/>
       <c r="B13" s="4"/>
       <c r="C13" s="13"/>
@@ -2027,7 +2379,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A14" s="5"/>
       <c r="B14" s="4"/>
       <c r="C14" s="13"/>
@@ -2035,7 +2387,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A15" s="5"/>
       <c r="B15" s="4"/>
       <c r="C15" s="13"/>
@@ -2043,7 +2395,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A16" s="5"/>
       <c r="B16" s="4"/>
       <c r="C16" s="13"/>
@@ -2051,7 +2403,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A17" s="5"/>
       <c r="B17" s="4"/>
       <c r="C17" s="13"/>
@@ -2059,7 +2411,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A18" s="5"/>
       <c r="B18" s="4"/>
       <c r="C18" s="13"/>
@@ -2067,7 +2419,7 @@
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A19" s="5"/>
       <c r="B19" s="4"/>
       <c r="C19" s="13"/>
@@ -2075,7 +2427,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A20" s="5"/>
       <c r="B20" s="4"/>
       <c r="C20" s="13"/>
@@ -2083,7 +2435,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A21" s="5"/>
       <c r="B21" s="4"/>
       <c r="C21" s="13"/>
@@ -2091,7 +2443,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A22" s="5"/>
       <c r="B22" s="4"/>
       <c r="C22" s="13"/>
@@ -2099,7 +2451,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A23" s="5"/>
       <c r="B23" s="4"/>
       <c r="C23" s="13"/>
@@ -2107,7 +2459,7 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A24" s="5"/>
       <c r="B24" s="4"/>
       <c r="C24" s="13"/>
@@ -2115,7 +2467,7 @@
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A25" s="5"/>
       <c r="B25" s="4"/>
       <c r="C25" s="13"/>
@@ -2123,7 +2475,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A26" s="10"/>
       <c r="B26" s="7"/>
       <c r="C26" s="13"/>
@@ -2131,7 +2483,7 @@
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A27" s="10"/>
       <c r="B27" s="7"/>
       <c r="C27" s="13"/>
@@ -2139,7 +2491,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A28" s="10"/>
       <c r="B28" s="7"/>
       <c r="C28" s="13"/>
@@ -2147,7 +2499,7 @@
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A29" s="10"/>
       <c r="B29" s="7"/>
       <c r="C29" s="13"/>
@@ -2155,7 +2507,7 @@
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15.3" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="10"/>
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
@@ -2163,7 +2515,7 @@
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.5">
       <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
@@ -2183,9 +2535,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2321,19 +2676,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE3BC1E-8E81-48D5-8B15-DA8BB79CB08C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5931B1-D6A7-4A49-B94B-92EB0E0D58B5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2357,9 +2708,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E5931B1-D6A7-4A49-B94B-92EB0E0D58B5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE3BC1E-8E81-48D5-8B15-DA8BB79CB08C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>